<commit_message>
Update DateBase/orders/Fresh bloom Flowers_2025-11-1.xlsx
</commit_message>
<xml_diff>
--- a/DateBase/orders/Fresh bloom Flowers_2025-11-1.xlsx
+++ b/DateBase/orders/Fresh bloom Flowers_2025-11-1.xlsx
@@ -778,6 +778,9 @@
       <c r="C41" t="str">
         <v>721_银扇干花_undefined_undefined_1bunch</v>
       </c>
+      <c r="F41" t="str">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <ignoredErrors>
@@ -839,7 +842,7 @@
         <v>0.00</v>
       </c>
       <c r="G2" t="str">
-        <v>0151540401033532151014713101491410105510115111082615151515151041590</v>
+        <v>01515404010335321510147131014914101055101151110826151515151510415950</v>
       </c>
     </row>
   </sheetData>

</xml_diff>